<commit_message>
information section is working - also fixed error on nav
</commit_message>
<xml_diff>
--- a/resources/MiscStuff/calculations.xlsx
+++ b/resources/MiscStuff/calculations.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,11 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/12a1b6a84f9f3060/WebProjects/SecretAgentSupply/resources/MiscStuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="30" documentId="7EC828CB8F89FE5CFB79F9DB2EA2EA0061B86E78" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{A643CA9F-5402-4D5B-871D-1ABE2C223002}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="21640" windowHeight="10790" xr2:uid="{5C4E3993-BB98-4620-B2A5-CC946B5A40DE}"/>
+    <workbookView xWindow="2800" yWindow="0" windowWidth="21640" windowHeight="10790" activeTab="1" xr2:uid="{5C4E3993-BB98-4620-B2A5-CC946B5A40DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Product" sheetId="1" r:id="rId1"/>
+    <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>px</t>
   </si>
@@ -57,6 +59,9 @@
   </si>
   <si>
     <t>Height</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -413,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855F0134-4C39-4DF6-ACC8-EDCEFDDAF284}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,4 +699,100 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8627B2-8A8C-430A-BA71-8F14B50B9FE6}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>960</v>
+      </c>
+      <c r="E2">
+        <f>$D$2*0.35</f>
+        <v>336</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>G2*$B$2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <f>$D$2*0.35</f>
+        <v>336</v>
+      </c>
+      <c r="G3">
+        <f>ROUND(1-SUM(I2:I4)/E2,2)*100</f>
+        <v>79</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f>G4*$B$2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <f>SUM(E2:E4)</f>
+        <v>672</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <f>(D2-D5)</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <f>SUM(E2:E7)</f>
+        <v>960</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>